<commit_message>
Fix validation set (7035 isolates)
</commit_message>
<xml_diff>
--- a/MCR_Analysis/mcr_rules_comparison.xlsx
+++ b/MCR_Analysis/mcr_rules_comparison.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/ecoli_amr_persistence/MCR_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA8D2814-E8A6-734D-B8DA-8B913044F5DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D26C4-1926-BB4D-9C98-1A88F84565C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" xr2:uid="{7AF115DE-9CAD-3B46-A9F6-E6AB510DBB1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>lhs</t>
   </si>
@@ -198,25 +198,40 @@
     <t>TRAINING SET</t>
   </si>
   <si>
-    <t>aadA1,aadA2,blaEC,cmlA1,dfrA12,floR,qacL,sul3</t>
-  </si>
-  <si>
-    <t>aadA1,aadA2,blaEC,cmlA1,dfrA12,floR,qacL,tet(A)</t>
-  </si>
-  <si>
-    <t>aph(3'')-Ib,aph(6)-Id,blaEC,floR,fosA3,mph(A),qacEdelta1,sul2,tet(A)</t>
-  </si>
-  <si>
-    <t>aadA1,aadA2,blaEC,cmlA1,dfrA12,floR,qacL,sul3,tet(A)</t>
-  </si>
-  <si>
     <t>VALIDATION SET</t>
   </si>
   <si>
-    <t>Not In Training Rules</t>
-  </si>
-  <si>
     <t>Match ID?</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,ble,dfrA12,qacEdelta1,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,blaEC,ble,dfrA12,qacEdelta1,sul1,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,blaEC,ble,dfrA12,qacEdelta1,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(6)-Id,blaEC,ble,dfrA12,qacEdelta1,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,blaEC,ble,dfrA12,qacEdelta1,sul1,sul2</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,blaEC,ble,dfrA12,qacEdelta1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,blaEC,ble,dfrA12,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aph(3'')-Ib,aph(6)-Id,blaEC,ble,dfrA12,qacEdelta1,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>aadA2,aph(3'')-Ib,aph(6)-Id,blaEC,ble,qacEdelta1,sul1,sul2,tet(A)</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -358,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -366,7 +381,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,15 +403,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,96 +722,96 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="10.83203125" style="2"/>
     <col min="9" max="9" width="58.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" customHeight="1" thickBot="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="13">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="K2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="L2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="M2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="N2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="O2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="P2" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -816,18 +828,41 @@
       <c r="G3" s="2">
         <v>39.952460823309501</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>108</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="P3" s="3"/>
+      <c r="I3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>95.067567567567593</v>
+      </c>
+      <c r="O3" s="2">
+        <v>7</v>
+      </c>
+      <c r="P3" s="3" t="e">
+        <f>VLOOKUP(I3,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -844,18 +879,41 @@
       <c r="G4" s="2">
         <v>38.301359962752201</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>119</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="P4" s="3"/>
+      <c r="I4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="N4" s="2">
+        <v>83.1841216216216</v>
+      </c>
+      <c r="O4" s="2">
+        <v>7</v>
+      </c>
+      <c r="P4" s="3" t="e">
+        <f>VLOOKUP(I4,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -872,18 +930,41 @@
       <c r="G5" s="2">
         <v>38.428961331033399</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>114</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="P5" s="3"/>
+      <c r="I5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="2">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>95.067567567567593</v>
+      </c>
+      <c r="O5" s="2">
+        <v>7</v>
+      </c>
+      <c r="P5" s="3" t="e">
+        <f>VLOOKUP(I5,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -900,18 +981,41 @@
       <c r="G6" s="2">
         <v>37.979499794997899</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>110</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="P6" s="3"/>
+      <c r="I6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>10</v>
+      </c>
+      <c r="L6" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="N6" s="2">
+        <v>83.1841216216216</v>
+      </c>
+      <c r="O6" s="2">
+        <v>7</v>
+      </c>
+      <c r="P6" s="3" t="e">
+        <f>VLOOKUP(I6,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -928,18 +1032,41 @@
       <c r="G7" s="2">
         <v>37.979499794997899</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>108</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="P7" s="3"/>
+      <c r="I7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="2">
+        <v>10</v>
+      </c>
+      <c r="L7" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="N7" s="2">
+        <v>73.941441441441398</v>
+      </c>
+      <c r="O7" s="2">
+        <v>7</v>
+      </c>
+      <c r="P7" s="3" t="e">
+        <f>VLOOKUP(I7,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -956,18 +1083,41 @@
       <c r="G8" s="2">
         <v>38.219876375978998</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>106</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="P8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10</v>
+      </c>
+      <c r="L8" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>95.067567567567593</v>
+      </c>
+      <c r="O8" s="2">
+        <v>7</v>
+      </c>
+      <c r="P8" s="3" t="e">
+        <f>VLOOKUP(I8,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -984,18 +1134,41 @@
       <c r="G9" s="2">
         <v>44.6913941553209</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>91</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="P9" s="3"/>
+      <c r="I9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10</v>
+      </c>
+      <c r="L9" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <v>95.067567567567593</v>
+      </c>
+      <c r="O9" s="2">
+        <v>7</v>
+      </c>
+      <c r="P9" s="3" t="e">
+        <f>VLOOKUP(I9,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -1012,18 +1185,41 @@
       <c r="G10" s="2">
         <v>45.460310360679401</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>79</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="1">
+      <c r="I10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="L10" s="2">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>95.067567567567593</v>
+      </c>
+      <c r="O10" s="2">
+        <v>7</v>
+      </c>
+      <c r="P10" s="3" t="e">
+        <f>VLOOKUP(I10,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17" thickBot="1">
+      <c r="A11" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -1040,18 +1236,41 @@
       <c r="G11" s="2">
         <v>39.289137718963403</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>80</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="P11" s="3"/>
+      <c r="I11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="5">
+        <v>10</v>
+      </c>
+      <c r="L11" s="5">
+        <v>9.9502487562189005E-4</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="N11" s="5">
+        <v>83.1841216216216</v>
+      </c>
+      <c r="O11" s="5">
+        <v>7</v>
+      </c>
+      <c r="P11" s="6" t="e">
+        <f>VLOOKUP(I11,A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
@@ -1068,18 +1287,17 @@
       <c r="G12" s="2">
         <v>40.396377054679597</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>78</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
@@ -1096,40 +1314,17 @@
       <c r="G13" s="2">
         <v>38.102809859267403</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <v>103</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="2">
-        <v>9</v>
-      </c>
-      <c r="L13" s="2">
-        <v>2.3666056832105302E-3</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.69117647058823495</v>
-      </c>
-      <c r="N13" s="2">
-        <v>37.199279982995897</v>
-      </c>
-      <c r="O13" s="2">
-        <v>141</v>
-      </c>
-      <c r="P13" s="3">
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
@@ -1146,18 +1341,17 @@
       <c r="G14" s="2">
         <v>37.979499794997899</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <v>90</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="P14" s="3"/>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
@@ -1174,18 +1368,17 @@
       <c r="G15" s="2">
         <v>46.419388638330801</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <v>66</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="P15" s="3"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1202,18 +1395,17 @@
       <c r="G16" s="2">
         <v>44.383020109270902</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>67</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="P16" s="3"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
@@ -1230,18 +1422,17 @@
       <c r="G17" s="2">
         <v>43.405142622854797</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <v>64</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1258,40 +1449,17 @@
       <c r="G18" s="2">
         <v>40.250013369698898</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <v>65</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="2">
-        <v>10</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1.5609526846707699E-3</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0.71538461538461495</v>
-      </c>
-      <c r="N18" s="2">
-        <v>38.502168021680198</v>
-      </c>
-      <c r="O18" s="2">
-        <v>93</v>
-      </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1308,40 +1476,17 @@
       <c r="G19" s="2">
         <v>38.762582264997903</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="3">
         <v>66</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" s="2">
-        <v>10</v>
-      </c>
-      <c r="L19" s="2">
-        <v>1.71201262189698E-3</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0.69387755102040805</v>
-      </c>
-      <c r="N19" s="2">
-        <v>37.3446527662555</v>
-      </c>
-      <c r="O19" s="2">
-        <v>102</v>
-      </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1">
         <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1358,40 +1503,17 @@
       <c r="G20" s="2">
         <v>41.042362681691301</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <v>67</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="2">
-        <v>10</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1.5609526846707699E-3</v>
-      </c>
-      <c r="M20" s="2">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="N20" s="2">
-        <v>40.042254742547399</v>
-      </c>
-      <c r="O20" s="2">
-        <v>93</v>
-      </c>
-      <c r="P20" s="3">
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1">
         <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1408,40 +1530,17 @@
       <c r="G21" s="2">
         <v>39.166359163591601</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="3">
         <v>66</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="2">
-        <v>10</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1.61130599707951E-3</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0.70072992700729897</v>
-      </c>
-      <c r="N21" s="2">
-        <v>37.7134492512808</v>
-      </c>
-      <c r="O21" s="2">
-        <v>96</v>
-      </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1458,18 +1557,17 @@
       <c r="G22" s="2">
         <v>37.979499794997899</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>66</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="P22" s="3"/>
+      <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B23" s="1">
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -1486,18 +1584,17 @@
       <c r="G23" s="2">
         <v>55.757137996911901</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <v>46</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="P23" s="3"/>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
@@ -1514,18 +1611,17 @@
       <c r="G24" s="2">
         <v>48.423862238622398</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="3">
         <v>51</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
@@ -1542,18 +1638,17 @@
       <c r="G25" s="2">
         <v>48.973565525128897</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>49</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="P25" s="3"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="B26" s="1">
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>8</v>
@@ -1570,18 +1665,17 @@
       <c r="G26" s="2">
         <v>52.5010732460266</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>47</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="P26" s="3"/>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="B27" s="1">
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
@@ -1598,18 +1692,17 @@
       <c r="G27" s="2">
         <v>49.2446056663956</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <v>51</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="P27" s="3"/>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="B28" s="1">
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>8</v>
@@ -1626,18 +1719,17 @@
       <c r="G28" s="2">
         <v>52.586999716150999</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>48</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="P28" s="3"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>8</v>
@@ -1654,18 +1746,17 @@
       <c r="G29" s="2">
         <v>49.4978726836449</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <v>53</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="P29" s="3"/>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -1682,18 +1773,17 @@
       <c r="G30" s="2">
         <v>52.669683677968898</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <v>49</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="P30" s="3"/>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B31" s="1">
+        <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -1710,18 +1800,17 @@
       <c r="G31" s="2">
         <v>48.973565525128897</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <v>49</v>
       </c>
-      <c r="I31" s="1"/>
-      <c r="P31" s="3"/>
+      <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="B32" s="1">
+        <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -1738,18 +1827,17 @@
       <c r="G32" s="2">
         <v>52.411709717097203</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <v>46</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="P32" s="3"/>
+      <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="B33" s="1">
+        <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
@@ -1766,18 +1854,17 @@
       <c r="G33" s="2">
         <v>50.395874727977997</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <v>46</v>
       </c>
-      <c r="I33" s="1"/>
-      <c r="P33" s="3"/>
+      <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B34" s="1">
+        <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>8</v>
@@ -1794,18 +1881,17 @@
       <c r="G34" s="2">
         <v>48.067804428044298</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>54</v>
       </c>
-      <c r="I34" s="1"/>
-      <c r="P34" s="3"/>
+      <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="B35" s="1">
+        <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>8</v>
@@ -1822,18 +1908,17 @@
       <c r="G35" s="2">
         <v>50.5199006707048</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>47</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="P35" s="3"/>
+      <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="B36" s="1">
+        <v>34</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>8</v>
@@ -1850,18 +1935,17 @@
       <c r="G36" s="2">
         <v>43.676424764247599</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <v>46</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="P36" s="3"/>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="B37" s="1">
+        <v>35</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
@@ -1878,18 +1962,17 @@
       <c r="G37" s="2">
         <v>47.926511646068803</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>53</v>
       </c>
-      <c r="I37" s="1"/>
-      <c r="P37" s="3"/>
+      <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>8</v>
@@ -1906,18 +1989,17 @@
       <c r="G38" s="2">
         <v>48.529360849164</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <v>46</v>
       </c>
-      <c r="I38" s="1"/>
-      <c r="P38" s="3"/>
+      <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="B39" s="1">
+        <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>8</v>
@@ -1934,18 +2016,17 @@
       <c r="G39" s="2">
         <v>48.973565525128897</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <v>49</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="P39" s="3"/>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="B40" s="1">
+        <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
@@ -1962,18 +2043,17 @@
       <c r="G40" s="2">
         <v>52.5010732460266</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <v>47</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="P40" s="3"/>
+      <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="B41" s="1">
+        <v>39</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>8</v>
@@ -1990,18 +2070,17 @@
       <c r="G41" s="2">
         <v>48.973565525128897</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <v>49</v>
       </c>
-      <c r="I41" s="1"/>
-      <c r="P41" s="3"/>
+      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="B42" s="1">
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
@@ -2018,18 +2097,17 @@
       <c r="G42" s="2">
         <v>50.093650591678298</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>51</v>
       </c>
-      <c r="I42" s="1"/>
-      <c r="P42" s="3"/>
+      <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="B43" s="1">
+        <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -2046,18 +2124,17 @@
       <c r="G43" s="2">
         <v>40.383265604807903</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>56</v>
       </c>
-      <c r="I43" s="1"/>
-      <c r="P43" s="3"/>
+      <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="B44" s="1">
+        <v>42</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
@@ -2074,40 +2151,17 @@
       <c r="G44" s="2">
         <v>38.657705148480098</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <v>57</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K44" s="2">
-        <v>11</v>
-      </c>
-      <c r="L44" s="2">
-        <v>1.4602460598532999E-3</v>
-      </c>
-      <c r="M44" s="2">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="N44" s="2">
-        <v>37.458883468834699</v>
-      </c>
-      <c r="O44" s="2">
-        <v>87</v>
-      </c>
-      <c r="P44" s="3">
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="1">
         <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>8</v>
@@ -2124,18 +2178,17 @@
       <c r="G45" s="2">
         <v>39.113216206788898</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
         <v>46</v>
       </c>
-      <c r="I45" s="1"/>
-      <c r="P45" s="3"/>
+      <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>8</v>
@@ -2152,18 +2205,17 @@
       <c r="G46" s="2">
         <v>55.386770534371998</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="3">
         <v>35</v>
       </c>
-      <c r="I46" s="1"/>
-      <c r="P46" s="3"/>
+      <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
@@ -2180,18 +2232,17 @@
       <c r="G47" s="2">
         <v>50.9724865669709</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
         <v>34</v>
       </c>
-      <c r="I47" s="1"/>
-      <c r="P47" s="3"/>
+      <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" ht="17" thickBot="1">
-      <c r="A48" s="4">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>53</v>
+      </c>
+      <c r="B48" s="4">
+        <v>46</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>8</v>
@@ -2208,115 +2259,22 @@
       <c r="G48" s="5">
         <v>39.529683460099903</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48" s="6">
         <v>34</v>
       </c>
-      <c r="I48" s="1"/>
-      <c r="P48" s="3"/>
-    </row>
-    <row r="49" spans="9:16">
-      <c r="I49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K49" s="2">
-        <v>9</v>
-      </c>
-      <c r="L49" s="2">
-        <v>2.50088118296715E-3</v>
-      </c>
-      <c r="M49" s="2">
-        <v>0.67420814479638003</v>
-      </c>
-      <c r="N49" s="2">
-        <v>36.286040703544302</v>
-      </c>
-      <c r="O49" s="2">
-        <v>149</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="9:16">
-      <c r="I50" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K50" s="2">
-        <v>9</v>
-      </c>
-      <c r="L50" s="2">
-        <v>2.38339012068011E-3</v>
-      </c>
-      <c r="M50" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="N50" s="2">
-        <v>35.880156579343598</v>
-      </c>
-      <c r="O50" s="2">
-        <v>142</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="9:16">
-      <c r="I51" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K51" s="2">
-        <v>10</v>
-      </c>
-      <c r="L51" s="2">
-        <v>1.6616593094882399E-3</v>
-      </c>
-      <c r="M51" s="2">
-        <v>0.68275862068965498</v>
-      </c>
-      <c r="N51" s="2">
-        <v>36.746229324362197</v>
-      </c>
-      <c r="O51" s="2">
-        <v>99</v>
-      </c>
-      <c r="P51" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="9:16" ht="17" thickBot="1">
-      <c r="I52" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K52" s="5">
-        <v>10</v>
-      </c>
-      <c r="L52" s="5">
-        <v>2.18197687104517E-3</v>
-      </c>
-      <c r="M52" s="5">
-        <v>0.68421052631578905</v>
-      </c>
-      <c r="N52" s="5">
-        <v>36.824371226168402</v>
-      </c>
-      <c r="O52" s="5">
-        <v>130</v>
-      </c>
-      <c r="P52" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="16:16">
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="16:16">
+      <c r="P50" s="2"/>
+    </row>
+    <row r="51" spans="16:16">
+      <c r="P51" s="2"/>
+    </row>
+    <row r="52" spans="16:16">
+      <c r="P52" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>